<commit_message>
feature biotype extraction from gencode gtf
</commit_message>
<xml_diff>
--- a/inst/extdata/tcga-barcode-codebook.xlsx
+++ b/inst/extdata/tcga-barcode-codebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lianoglou/workspace/projects/FacileData/datasets/FacileTcgaDataSet/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25A97A7-5515-1D47-9D9C-05FB9904E1A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC7C4BB-EC94-1D4A-ACA5-99146071E576}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6880" yWindow="560" windowWidth="28040" windowHeight="17040" xr2:uid="{599D40BA-27E8-CC4B-8EF7-0AF9A2FFD2F8}"/>
+    <workbookView xWindow="8840" yWindow="3400" windowWidth="28040" windowHeight="17040" xr2:uid="{599D40BA-27E8-CC4B-8EF7-0AF9A2FFD2F8}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="3" r:id="rId1"/>
@@ -3981,9 +3981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BBA1F3-49AE-A746-A1E0-40E9CDA165E4}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -4134,7 +4132,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A11" sqref="A11:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4480,9 +4478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60E5CBEE-F330-F349-8B3E-3B2F0D265100}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -4580,6 +4576,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>